<commit_message>
Fin du cours 27.02.2017
Création base de données + insertion données
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>Adaptation du template suppression de ce que je n'utilise pas + documentation</t>
+  </si>
+  <si>
+    <t>Maladie</t>
+  </si>
+  <si>
+    <t>Exportation de la base de donnée pas terminé + création script création donnée + db</t>
+  </si>
+  <si>
+    <t>1'000 données de chaque types ont été crées</t>
+  </si>
+  <si>
+    <t>Correction MLD (envoyé le 08.02 et le 09.02) + création base de données</t>
+  </si>
+  <si>
+    <t>Base de données crée + insertion de données OK + lecture openclasseroom modèle MVC</t>
   </si>
 </sst>
 </file>
@@ -299,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -364,61 +379,76 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -704,8 +734,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,35 +763,35 @@
       <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="11">
         <v>43130</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="38"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="12">
@@ -770,15 +800,15 @@
       <c r="C5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="12">
@@ -787,13 +817,13 @@
       <c r="C6" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="33"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="12">
@@ -802,13 +832,13 @@
       <c r="C7" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="33"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F7" s="32"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="12">
@@ -817,13 +847,13 @@
       <c r="C8" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="32"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -832,35 +862,35 @@
       <c r="B9" s="25">
         <v>43139</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="13">
         <v>43140</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="34"/>
-      <c r="H10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
@@ -869,26 +899,28 @@
       <c r="C11" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="33"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="32"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>43144</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="33"/>
+      <c r="C12" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="34"/>
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F12" s="32"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -897,27 +929,31 @@
       <c r="B13" s="26">
         <v>43146</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="33"/>
+      <c r="C13" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="34"/>
       <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="32"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="34"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="12">
         <v>43147</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
+      <c r="C14" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="34"/>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F14" s="32"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
@@ -930,32 +966,40 @@
       <c r="G15" s="6"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="12">
+    <row r="16" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="28">
         <v>43157</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="33"/>
+      <c r="C16" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="38"/>
+      <c r="E16" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="12">
         <v>43158</v>
       </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+      <c r="C17" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="38"/>
       <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="33"/>
+      <c r="F17" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -964,53 +1008,53 @@
       <c r="B18" s="25">
         <v>43160</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
       <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="32"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <v>43161</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="38"/>
       <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F19" s="32"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="12">
         <v>43164</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="29"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
       <c r="E20" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F20" s="32"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="12">
         <v>43165</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
       <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F21" s="32"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1019,54 +1063,54 @@
       <c r="B22" s="26">
         <v>43167</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38"/>
       <c r="E22" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="32"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="12">
         <v>43168</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="12">
         <v>43171</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="29"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
       <c r="E24" s="9" t="s">
         <v>5</v>
       </c>
       <c r="F24" s="32"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="34"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="13">
         <v>43172</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="10" t="s">
         <v>5</v>
       </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1075,53 +1119,53 @@
       <c r="B26" s="26">
         <v>43174</v>
       </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="29"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
       <c r="E26" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="32"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="13">
         <v>43175</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="38"/>
       <c r="E27" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F27" s="32"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="13">
         <v>43178</v>
       </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="29"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="38"/>
       <c r="E28" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F28" s="32"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="13">
         <v>43179</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="38"/>
       <c r="E29" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F29" s="32"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="34"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1130,53 +1174,53 @@
       <c r="B30" s="25">
         <v>43181</v>
       </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="38"/>
       <c r="E30" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F30" s="32"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="34"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="13">
         <v>43182</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
       <c r="E31" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F31" s="32"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="34"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" s="13">
         <v>43185</v>
       </c>
       <c r="C32" s="32"/>
-      <c r="D32" s="33"/>
+      <c r="D32" s="34"/>
       <c r="E32" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F32" s="32"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B33" s="13">
         <v>43186</v>
       </c>
       <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
+      <c r="D33" s="34"/>
       <c r="E33" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F33" s="32"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -1185,64 +1229,64 @@
       <c r="B34" s="25">
         <v>43188</v>
       </c>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
       <c r="E34" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F34" s="32"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B35" s="20">
         <v>43189</v>
       </c>
-      <c r="C35" s="46" t="s">
+      <c r="C35" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="36"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="34"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="20">
         <v>43205</v>
       </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="34"/>
-      <c r="H36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="34"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="17">
         <v>43206</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F37" s="32"/>
-      <c r="G37" s="34"/>
-      <c r="H37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="34"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38" s="18">
         <v>43207</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
+      <c r="C38" s="37"/>
+      <c r="D38" s="38"/>
       <c r="E38" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F38" s="32"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="34"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1251,27 +1295,27 @@
       <c r="B39" s="27">
         <v>43209</v>
       </c>
-      <c r="C39" s="28"/>
-      <c r="D39" s="29"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="38"/>
       <c r="E39" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F39" s="32"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="34"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="19">
         <v>43210</v>
       </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="44"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="31"/>
       <c r="E40" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="44"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="31"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -1280,52 +1324,17 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C35:E36"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F29:H29"/>
@@ -1342,17 +1351,52 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C35:E36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5:H5" r:id="rId1" display="Accessible ici"/>

</xml_diff>

<commit_message>
commit fin de la matinée
a push a midi
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Chez moi ou prochain cours index.php et les vues</t>
+  </si>
+  <si>
+    <t>login.php ne fonctionne a corriger</t>
+  </si>
+  <si>
+    <t>Page portfolio_modify.php presque finie (plus que exportation et importation données) + modele.php adaptation in progress + login.php in progress</t>
   </si>
 </sst>
 </file>
@@ -338,136 +344,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -482,6 +382,90 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -767,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23:H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,579 +776,611 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="A4" s="15"/>
+      <c r="B4" s="18">
         <v>43130</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="43" t="s">
+      <c r="D4" s="20"/>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="A5" s="15"/>
+      <c r="B5" s="3">
         <v>43132</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="48"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="12">
+      <c r="A6" s="15"/>
+      <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12">
+      <c r="A7" s="15"/>
+      <c r="B7" s="3">
         <v>43136</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="32"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="12">
+      <c r="A8" s="15"/>
+      <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="9"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="27">
         <v>43139</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="34"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="13">
+      <c r="A10" s="15"/>
+      <c r="B10" s="29">
         <v>43140</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="32" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="12">
+      <c r="A11" s="15"/>
+      <c r="B11" s="3">
         <v>43143</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="12">
+      <c r="A12" s="15"/>
+      <c r="B12" s="3">
         <v>43144</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="34"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="9"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="30">
         <v>43146</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="12">
+      <c r="A14" s="15"/>
+      <c r="B14" s="3">
         <v>43147</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="9"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="22" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="5"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="28">
+      <c r="A16" s="15"/>
+      <c r="B16" s="3">
         <v>43157</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="38"/>
-      <c r="E16" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="50" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="51"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="12">
+      <c r="A17" s="6"/>
+      <c r="B17" s="3">
         <v>43158</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="32" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="25">
+      <c r="B18" s="27">
         <v>43160</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="11"/>
+      <c r="E18" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="40"/>
-      <c r="H18" s="41"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12">
+      <c r="A19" s="15"/>
+      <c r="B19" s="3">
         <v>43161</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="39" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12">
+      <c r="A20" s="15"/>
+      <c r="B20" s="3">
         <v>43164</v>
       </c>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="32" t="s">
+      <c r="D20" s="11"/>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12">
+      <c r="A21" s="15"/>
+      <c r="B21" s="3">
         <v>43165</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="32" t="s">
+      <c r="D21" s="9"/>
+      <c r="E21" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="G21" s="26"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="30">
         <v>43167</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="10" t="s">
+      <c r="C22" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
+      <c r="F22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="26"/>
+      <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12">
+      <c r="A23" s="15"/>
+      <c r="B23" s="3">
         <v>43168</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="34"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="12">
+      <c r="A24" s="6"/>
+      <c r="B24" s="3">
         <v>43171</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="13">
+      <c r="A25" s="15"/>
+      <c r="B25" s="29">
         <v>43172</v>
       </c>
-      <c r="C25" s="53"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="34"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="30">
         <v>43174</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="10" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="34"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="9"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="13">
+      <c r="A27" s="15"/>
+      <c r="B27" s="29">
         <v>43175</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="34"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="13">
+      <c r="A28" s="15"/>
+      <c r="B28" s="29">
         <v>43178</v>
       </c>
-      <c r="C28" s="37"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="34"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="9"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="13">
+      <c r="A29" s="15"/>
+      <c r="B29" s="29">
         <v>43179</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="34"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="25">
+      <c r="B30" s="27">
         <v>43181</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="4" t="s">
+      <c r="C30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="13">
+      <c r="A31" s="15"/>
+      <c r="B31" s="29">
         <v>43182</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="34"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13">
+      <c r="A32" s="15"/>
+      <c r="B32" s="29">
         <v>43185</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="8"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="13">
+      <c r="A33" s="15"/>
+      <c r="B33" s="29">
         <v>43186</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="25">
+      <c r="B34" s="27">
         <v>43188</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="4" t="s">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="32"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="34"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="9"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="20">
+      <c r="A35" s="15"/>
+      <c r="B35" s="31">
         <v>43189</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="34"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="9"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="20">
+      <c r="A36" s="15"/>
+      <c r="B36" s="31">
         <v>43205</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="34"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="17">
+      <c r="A37" s="15"/>
+      <c r="B37" s="29">
         <v>43206</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="32"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="34"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="8"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="18">
+      <c r="A38" s="15"/>
+      <c r="B38" s="37">
         <v>43207</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="34"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="15" t="s">
         <v>15</v>
       </c>
       <c r="B39" s="27">
         <v>43209</v>
       </c>
-      <c r="C39" s="37"/>
-      <c r="D39" s="38"/>
-      <c r="E39" s="4" t="s">
+      <c r="C39" s="8"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
-      <c r="H39" s="34"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="19">
+      <c r="A40" s="15"/>
+      <c r="B40" s="38">
         <v>43210</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F40" s="30"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="31"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F40" s="39"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="40"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>

</xml_diff>

<commit_message>
Commit fin du cours 12.03.18
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="44">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>continuer le week-end</t>
+  </si>
+  <si>
+    <t>Debug de la fonction getLogin… + login.php</t>
+  </si>
+  <si>
+    <t>A la maison durant le week-end lecture du chapitres 5 à 14</t>
+  </si>
+  <si>
+    <t>Ce soir lecture openclassroom + essaie de dépannage</t>
   </si>
 </sst>
 </file>
@@ -414,25 +423,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -444,6 +447,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,13 +471,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -755,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:H20"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,6 +775,7 @@
     <col min="3" max="3" width="85.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
@@ -787,102 +797,102 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="32"/>
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="9">
         <v>43130</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>43132</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="38"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="24"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="27"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>43136</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="27"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="24"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="24"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -891,68 +901,68 @@
       <c r="B9" s="11">
         <v>43139</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="27"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="24"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="12">
         <v>43140</v>
       </c>
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="26"/>
-      <c r="H10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>43143</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="27"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="27"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="24"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>43144</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="27"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="27"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="24"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -961,32 +971,32 @@
       <c r="B13" s="13">
         <v>43146</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3">
         <v>43147</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="24"/>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="27"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -1005,292 +1015,299 @@
       <c r="B16" s="3">
         <v>43157</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="27"/>
+      <c r="D16" s="24"/>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="29"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>43158</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="26"/>
-      <c r="H17" s="27"/>
-    </row>
-    <row r="18" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="27"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="11">
         <v>43160</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="32"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
-    </row>
-    <row r="19" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="29"/>
+      <c r="H18" s="30"/>
+    </row>
+    <row r="19" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3">
         <v>43161</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="27"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
-    </row>
-    <row r="20" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="29"/>
+      <c r="H19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3">
         <v>43164</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="32"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G20" s="27"/>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="3">
         <v>43165</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="27"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
-    </row>
-    <row r="22" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="27"/>
+      <c r="H21" s="24"/>
+    </row>
+    <row r="22" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="13">
         <v>43167</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="32"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G22" s="29"/>
+      <c r="H22" s="30"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="3">
         <v>43168</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="27"/>
+      <c r="H23" s="24"/>
+      <c r="I23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="3">
         <v>43171</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="27"/>
+      <c r="C24" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="24"/>
       <c r="E24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F24" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G24" s="27"/>
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="12">
         <v>43172</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="42"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F25" s="23"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="13">
         <v>43174</v>
       </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="27"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
       <c r="E26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="27"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="23"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="12">
         <v>43175</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="27"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="24"/>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="27"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F27" s="23"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="12">
         <v>43178</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="27"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
       <c r="E28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="27"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F28" s="23"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="12">
         <v>43179</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="27"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
       <c r="E29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="25"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="27"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F29" s="23"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="24"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="11">
         <v>43181</v>
       </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="27"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
       <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="27"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F30" s="23"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="12">
         <v>43182</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F31" s="23"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="12">
         <v>43185</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="27"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
       <c r="E32" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="27"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="24"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="12">
         <v>43186</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="27"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
       <c r="E33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="27"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="24"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -1299,68 +1316,68 @@
       <c r="B34" s="11">
         <v>43188</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="27"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="24"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="14">
         <v>43189</v>
       </c>
-      <c r="C35" s="29" t="s">
+      <c r="C35" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="24"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="14">
         <v>43205</v>
       </c>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="27"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="24"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="12">
         <v>43206</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="27"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="24"/>
       <c r="E37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="27"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="24"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="20">
         <v>43207</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="27"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="24"/>
       <c r="E38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="25"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="27"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1369,28 +1386,28 @@
       <c r="B39" s="11">
         <v>43209</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="27"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="25"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="27"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="24"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="21">
         <v>43210</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
       <c r="E40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="23"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="24"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="41"/>
+      <c r="H40" s="40"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -1399,17 +1416,52 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F29:H29"/>
@@ -1426,52 +1478,17 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5:H5" r:id="rId1" display="Accessible ici"/>

</xml_diff>

<commit_message>
commit doc + debug login
documentation + debug de la fonction login
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>corrections de requêtes dans modele.php + erreur contrôleur.php envoie page portfolio.php</t>
+  </si>
+  <si>
+    <t>corriger des erreurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">documentation + debug </t>
   </si>
 </sst>
 </file>
@@ -444,19 +450,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -468,44 +483,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -791,7 +797,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D27"/>
+      <selection activeCell="C28" sqref="C28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,102 +827,102 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="32" t="s">
+      <c r="F3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="9">
         <v>43130</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="34"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>43132</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="28"/>
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="24"/>
+      <c r="D6" s="28"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="27"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="28"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>43136</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="24"/>
+      <c r="D7" s="28"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="27"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="28"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="28"/>
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="27"/>
-      <c r="H8" s="24"/>
+      <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -925,68 +931,68 @@
       <c r="B9" s="11">
         <v>43139</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="26" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="27"/>
-      <c r="H9" s="24"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="12">
         <v>43140</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="26" t="s">
         <v>21</v>
       </c>
       <c r="G10" s="27"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>43143</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="24"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="27"/>
-      <c r="H11" s="24"/>
+      <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>43144</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="24"/>
+      <c r="D12" s="28"/>
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="23"/>
+      <c r="F12" s="26"/>
       <c r="G12" s="27"/>
-      <c r="H12" s="24"/>
+      <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -995,32 +1001,32 @@
       <c r="B13" s="13">
         <v>43146</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="24"/>
+      <c r="D13" s="28"/>
       <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="23"/>
+      <c r="F13" s="26"/>
       <c r="G13" s="27"/>
-      <c r="H13" s="24"/>
+      <c r="H13" s="28"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3">
         <v>43147</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="24"/>
+      <c r="D14" s="28"/>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="23"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="27"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="28"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -1039,36 +1045,36 @@
       <c r="B16" s="3">
         <v>43157</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="24"/>
+      <c r="D16" s="28"/>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="29"/>
-      <c r="H16" s="30"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>43158</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="28"/>
       <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="26" t="s">
         <v>26</v>
       </c>
       <c r="G17" s="27"/>
-      <c r="H17" s="24"/>
+      <c r="H17" s="28"/>
     </row>
     <row r="18" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1077,72 +1083,72 @@
       <c r="B18" s="11">
         <v>43160</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="33"/>
       <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="29"/>
-      <c r="H18" s="30"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
     </row>
     <row r="19" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3">
         <v>43161</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="24"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="28" t="s">
+      <c r="F19" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="29"/>
-      <c r="H19" s="30"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="33"/>
     </row>
     <row r="20" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3">
         <v>43164</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="30"/>
+      <c r="D20" s="33"/>
       <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="23" t="s">
+      <c r="F20" s="26" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="27"/>
-      <c r="H20" s="24"/>
+      <c r="H20" s="28"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="3">
         <v>43165</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="24"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="26" t="s">
         <v>36</v>
       </c>
       <c r="G21" s="27"/>
-      <c r="H21" s="24"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -1151,36 +1157,36 @@
       <c r="B22" s="13">
         <v>43167</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="30"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="28" t="s">
+      <c r="F22" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="29"/>
-      <c r="H22" s="30"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="3">
         <v>43168</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="24"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="26" t="s">
         <v>40</v>
       </c>
       <c r="G23" s="27"/>
-      <c r="H23" s="24"/>
+      <c r="H23" s="28"/>
       <c r="I23" t="s">
         <v>42</v>
       </c>
@@ -1190,18 +1196,18 @@
       <c r="B24" s="3">
         <v>43171</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="24"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="26" t="s">
         <v>43</v>
       </c>
       <c r="G24" s="27"/>
-      <c r="H24" s="24"/>
+      <c r="H24" s="28"/>
       <c r="I24" t="s">
         <v>44</v>
       </c>
@@ -1211,16 +1217,16 @@
       <c r="B25" s="12">
         <v>43172</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="43"/>
       <c r="E25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="23"/>
+      <c r="F25" s="26"/>
       <c r="G25" s="27"/>
-      <c r="H25" s="24"/>
+      <c r="H25" s="28"/>
     </row>
     <row r="26" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1229,19 +1235,19 @@
       <c r="B26" s="13">
         <v>43174</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="24"/>
+      <c r="D26" s="28"/>
       <c r="E26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="29"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="43" t="s">
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+      <c r="I26" s="23" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1250,46 +1256,50 @@
       <c r="B27" s="12">
         <v>43175</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="24"/>
+      <c r="D27" s="28"/>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="23" t="s">
+      <c r="F27" s="26" t="s">
         <v>49</v>
       </c>
       <c r="G27" s="27"/>
-      <c r="H27" s="24"/>
+      <c r="H27" s="28"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="12">
         <v>43178</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="24"/>
+      <c r="C28" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="28"/>
       <c r="E28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="23"/>
+      <c r="F28" s="26" t="s">
+        <v>51</v>
+      </c>
       <c r="G28" s="27"/>
-      <c r="H28" s="24"/>
+      <c r="H28" s="28"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="12">
         <v>43179</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="23"/>
+      <c r="F29" s="26"/>
       <c r="G29" s="27"/>
-      <c r="H29" s="24"/>
+      <c r="H29" s="28"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1298,14 +1308,14 @@
       <c r="B30" s="11">
         <v>43181</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="24"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="28"/>
       <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="23"/>
+      <c r="F30" s="26"/>
       <c r="G30" s="27"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="28"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
@@ -1317,37 +1327,37 @@
       <c r="E31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="23"/>
+      <c r="F31" s="26"/>
       <c r="G31" s="27"/>
-      <c r="H31" s="24"/>
+      <c r="H31" s="28"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="12">
         <v>43185</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="24"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="28"/>
       <c r="E32" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="27"/>
-      <c r="H32" s="24"/>
+      <c r="H32" s="28"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="12">
         <v>43186</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="28"/>
       <c r="E33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="26"/>
       <c r="G33" s="27"/>
-      <c r="H33" s="24"/>
+      <c r="H33" s="28"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -1361,63 +1371,63 @@
       <c r="E34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="26"/>
       <c r="G34" s="27"/>
-      <c r="H34" s="24"/>
+      <c r="H34" s="28"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="14">
         <v>43189</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="23"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="26"/>
       <c r="G35" s="27"/>
-      <c r="H35" s="24"/>
+      <c r="H35" s="28"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="14">
         <v>43205</v>
       </c>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="23"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="27"/>
-      <c r="H36" s="24"/>
+      <c r="H36" s="28"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="12">
         <v>43206</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="28"/>
       <c r="E37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="23"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="27"/>
-      <c r="H37" s="24"/>
+      <c r="H37" s="28"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="20">
         <v>43207</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="24"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="28"/>
       <c r="E38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="23"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="27"/>
-      <c r="H38" s="24"/>
+      <c r="H38" s="28"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1426,28 +1436,28 @@
       <c r="B39" s="11">
         <v>43209</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="28"/>
       <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="23"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="27"/>
-      <c r="H39" s="24"/>
+      <c r="H39" s="28"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="21">
         <v>43210</v>
       </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="40"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="25"/>
       <c r="E40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="39"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="40"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="25"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -1456,52 +1466,17 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C35:E36"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F29:H29"/>
@@ -1518,17 +1493,52 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C35:E36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5:H5" r:id="rId1" display="Accessible ici"/>

</xml_diff>

<commit_message>
commit debug fonction chargement données
chargement des données à la page vue_portfolio.php
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t xml:space="preserve">documentation + debug </t>
+  </si>
+  <si>
+    <t>chargement des données sur la page portfolio.php + requêtes recherches de données</t>
+  </si>
+  <si>
+    <t>aide de raphael a faire encore envoyer les données</t>
   </si>
 </sst>
 </file>
@@ -453,25 +459,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -483,6 +483,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -504,13 +507,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -796,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:D28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,102 +833,102 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="9">
         <v>43130</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>43132</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>43136</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -931,68 +937,68 @@
       <c r="B9" s="11">
         <v>43139</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="12">
         <v>43140</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>43143</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>43144</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1001,32 +1007,32 @@
       <c r="B13" s="13">
         <v>43146</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3">
         <v>43147</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -1045,36 +1051,36 @@
       <c r="B16" s="3">
         <v>43157</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>43158</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1083,72 +1089,72 @@
       <c r="B18" s="11">
         <v>43160</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="33"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3">
         <v>43161</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="25"/>
       <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3">
         <v>43164</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="33"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="3">
         <v>43165</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -1157,36 +1163,36 @@
       <c r="B22" s="13">
         <v>43167</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="33"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="3">
         <v>43168</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="25"/>
       <c r="I23" t="s">
         <v>42</v>
       </c>
@@ -1196,18 +1202,18 @@
       <c r="B24" s="3">
         <v>43171</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="28"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="25"/>
       <c r="I24" t="s">
         <v>44</v>
       </c>
@@ -1217,16 +1223,16 @@
       <c r="B25" s="12">
         <v>43172</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="43"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="28"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1235,18 +1241,18 @@
       <c r="B26" s="13">
         <v>43174</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="28"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="32"/>
-      <c r="H26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="23" t="s">
         <v>48</v>
       </c>
@@ -1256,50 +1262,54 @@
       <c r="B27" s="12">
         <v>43175</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="12">
         <v>43178</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="25"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="12">
         <v>43179</v>
       </c>
-      <c r="C29" s="26"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="25"/>
       <c r="E29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="26"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="F29" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G29" s="28"/>
+      <c r="H29" s="25"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1308,56 +1318,56 @@
       <c r="B30" s="11">
         <v>43181</v>
       </c>
-      <c r="C30" s="26"/>
-      <c r="D30" s="28"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="26"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="25"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="12">
         <v>43182</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="25"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="12">
         <v>43185</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="28"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
       <c r="E32" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="25"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="12">
         <v>43186</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="28"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
       <c r="E33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="25"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -1366,68 +1376,68 @@
       <c r="B34" s="11">
         <v>43188</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
       <c r="E34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="28"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="14">
         <v>43189</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="28"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="25"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="14">
         <v>43205</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="28"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="25"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="12">
         <v>43206</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="28"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="25"/>
       <c r="E37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="26"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="28"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="25"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="20">
         <v>43207</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="28"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="25"/>
       <c r="E38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="25"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1436,28 +1446,28 @@
       <c r="B39" s="11">
         <v>43209</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="28"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="25"/>
       <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="28"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="25"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="21">
         <v>43210</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="41"/>
       <c r="E40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="25"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="41"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -1466,17 +1476,52 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F29:H29"/>
@@ -1493,52 +1538,17 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5:H5" r:id="rId1" display="Accessible ici"/>

</xml_diff>

<commit_message>
commit modèle + controleur
debugg vue_portfolio + modification dans modele.php et controleur.php avancement des vues_administrator
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>encore debugg</t>
+  </si>
+  <si>
+    <t>pas d'affichage sur vue_administrator.php pas encore d'envoie sur vue_portfolio.php</t>
+  </si>
+  <si>
+    <t>modele.php (nettoyage + debug) + controleur.php (nettoyage + debug) pour les pages vue_administrator.php et  vue_portfolio.php</t>
   </si>
 </sst>
 </file>
@@ -404,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -471,25 +477,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -501,6 +501,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -522,14 +525,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -814,14 +823,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33:H33"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36:H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="85.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
     <col min="8" max="8" width="33.28515625" customWidth="1"/>
     <col min="9" max="9" width="77.5703125" customWidth="1"/>
   </cols>
@@ -845,102 +854,102 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="34"/>
+      <c r="D3" s="33"/>
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="9">
         <v>43130</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="37"/>
-      <c r="H4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>43132</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="28"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="28"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>43136</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="28"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -949,68 +958,68 @@
       <c r="B9" s="11">
         <v>43139</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="28"/>
+      <c r="D9" s="25"/>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="12">
         <v>43140</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="28"/>
+      <c r="D10" s="25"/>
       <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="25"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>43143</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="28"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>43144</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="28"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1019,32 +1028,32 @@
       <c r="B13" s="13">
         <v>43146</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3">
         <v>43147</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="25"/>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -1063,36 +1072,36 @@
       <c r="B16" s="3">
         <v>43157</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="25"/>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="33"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>43158</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1101,72 +1110,72 @@
       <c r="B18" s="11">
         <v>43160</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="33"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3">
         <v>43161</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="25"/>
       <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="33"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3">
         <v>43164</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="33"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="3">
         <v>43165</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -1175,36 +1184,36 @@
       <c r="B22" s="13">
         <v>43167</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="33"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="3">
         <v>43168</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="26" t="s">
+      <c r="F23" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="25"/>
       <c r="I23" t="s">
         <v>42</v>
       </c>
@@ -1214,18 +1223,18 @@
       <c r="B24" s="3">
         <v>43171</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="28"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="26" t="s">
+      <c r="F24" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="25"/>
       <c r="I24" t="s">
         <v>44</v>
       </c>
@@ -1235,16 +1244,16 @@
       <c r="B25" s="12">
         <v>43172</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="43"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="28"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1253,18 +1262,18 @@
       <c r="B26" s="13">
         <v>43174</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="28"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="32"/>
-      <c r="H26" s="33"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="23" t="s">
         <v>48</v>
       </c>
@@ -1274,54 +1283,54 @@
       <c r="B27" s="12">
         <v>43175</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="12">
         <v>43178</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="26" t="s">
+      <c r="F28" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="25"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="12">
         <v>43179</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="28"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="26" t="s">
+      <c r="F29" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="25"/>
     </row>
     <row r="30" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1330,64 +1339,68 @@
       <c r="B30" s="11">
         <v>43181</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="33"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="12">
         <v>43182</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="27"/>
+      <c r="D31" s="28"/>
       <c r="E31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="26" t="s">
+      <c r="F31" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="28"/>
+      <c r="H31" s="25"/>
+    </row>
+    <row r="32" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="12">
         <v>43185</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F32" s="26"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
+      <c r="C32" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="31"/>
+      <c r="E32" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="12">
         <v>43186</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="28"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
       <c r="E33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="25"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -1396,68 +1409,68 @@
       <c r="B34" s="11">
         <v>43188</v>
       </c>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
       <c r="E34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="28"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="14">
         <v>43189</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="28"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="25"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="14">
         <v>43205</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="28"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="25"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="12">
         <v>43206</v>
       </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="28"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="25"/>
       <c r="E37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="26"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="28"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="25"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="20">
         <v>43207</v>
       </c>
-      <c r="C38" s="26"/>
-      <c r="D38" s="28"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="25"/>
       <c r="E38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="26"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="25"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -1466,28 +1479,28 @@
       <c r="B39" s="11">
         <v>43209</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="28"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="25"/>
       <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="26"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="28"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="25"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="21">
         <v>43210</v>
       </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="25"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="41"/>
       <c r="E40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="24"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="25"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="42"/>
+      <c r="H40" s="41"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -1496,17 +1509,52 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F29:H29"/>
@@ -1523,52 +1571,17 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5:H5" r:id="rId1" display="Accessible ici"/>

</xml_diff>

<commit_message>
Dernier commit projet Portfolio
document final avec documentation finale
</commit_message>
<xml_diff>
--- a/Projet Web/Documentation/Journal de travail Corentin.xlsx
+++ b/Projet Web/Documentation/Journal de travail Corentin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="74">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -234,6 +234,18 @@
   </si>
   <si>
     <t>Presque fini la doc manque manuel utilisation + conclusion</t>
+  </si>
+  <si>
+    <t>Durant temps libre manuel d'utilisation + création doc avec annexes</t>
+  </si>
+  <si>
+    <t>documentation partie conclusion</t>
+  </si>
+  <si>
+    <t>maladie</t>
+  </si>
+  <si>
+    <t>Objectifs, points positifs-négatifs, difficultés, suite, …</t>
   </si>
 </sst>
 </file>
@@ -507,35 +519,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -558,13 +567,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -851,7 +863,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40:D40"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,102 +893,102 @@
       <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="9">
         <v>43130</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="3">
         <v>43132</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="3">
         <v>43133</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="3">
         <v>43136</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="29"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="3">
         <v>43137</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -985,68 +997,68 @@
       <c r="B9" s="11">
         <v>43139</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="29"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="12">
         <v>43140</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="29"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>43143</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="29"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>43144</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="29"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="29"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="26"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1055,32 +1067,32 @@
       <c r="B13" s="13">
         <v>43146</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="29"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="3">
         <v>43147</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -1099,36 +1111,36 @@
       <c r="B16" s="3">
         <v>43157</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="31"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="3">
         <v>43158</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="18" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1137,72 +1149,72 @@
       <c r="B18" s="11">
         <v>43160</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="31"/>
       <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="32" t="s">
+      <c r="F18" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="3">
         <v>43161</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="26"/>
       <c r="E19" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="3">
         <v>43164</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="34"/>
+      <c r="D20" s="31"/>
       <c r="E20" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="26"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="3">
         <v>43165</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="26"/>
       <c r="E21" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="26"/>
     </row>
     <row r="22" spans="1:9" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -1211,36 +1223,36 @@
       <c r="B22" s="13">
         <v>43167</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="34"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="34"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="31"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="3">
         <v>43168</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="26"/>
       <c r="E23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="26"/>
       <c r="I23" t="s">
         <v>42</v>
       </c>
@@ -1250,18 +1262,18 @@
       <c r="B24" s="3">
         <v>43171</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="29"/>
+      <c r="D24" s="26"/>
       <c r="E24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="26"/>
       <c r="I24" t="s">
         <v>44</v>
       </c>
@@ -1271,16 +1283,16 @@
       <c r="B25" s="12">
         <v>43172</v>
       </c>
-      <c r="C25" s="43" t="s">
+      <c r="C25" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="44"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1289,18 +1301,18 @@
       <c r="B26" s="13">
         <v>43174</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="29"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="32" t="s">
+      <c r="F26" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="34"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="23" t="s">
         <v>66</v>
       </c>
@@ -1310,54 +1322,54 @@
       <c r="B27" s="12">
         <v>43175</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="26"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="12">
         <v>43178</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="26"/>
       <c r="E28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="26"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="12">
         <v>43179</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="26"/>
       <c r="E29" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="26"/>
     </row>
     <row r="30" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1366,72 +1378,72 @@
       <c r="B30" s="11">
         <v>43181</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="29"/>
+      <c r="D30" s="26"/>
       <c r="E30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="G30" s="33"/>
-      <c r="H30" s="34"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="31"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="12">
         <v>43182</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="28"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G31" s="28"/>
-      <c r="H31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="26"/>
     </row>
     <row r="32" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="12">
         <v>43185</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="34"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="32" t="s">
+      <c r="F32" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="34"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="31"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="12">
         <v>43186</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="33"/>
-      <c r="H33" s="34"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="31"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -1440,78 +1452,78 @@
       <c r="B34" s="11">
         <v>43188</v>
       </c>
-      <c r="C34" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="28"/>
+      <c r="C34" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="29"/>
       <c r="E34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="G34" s="28"/>
-      <c r="H34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="26"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="14">
         <v>43189</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="29"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="26"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="14">
         <v>43205</v>
       </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="29"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="26"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="12">
         <v>43206</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="26"/>
       <c r="E37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="27"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="29"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="20">
         <v>43207</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="29"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="27" t="s">
+      <c r="F38" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="28"/>
-      <c r="H38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="26"/>
       <c r="I38" t="s">
         <v>67</v>
       </c>
@@ -1523,32 +1535,39 @@
       <c r="B39" s="11">
         <v>43209</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D39" s="29"/>
+      <c r="D39" s="26"/>
       <c r="E39" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F39" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="G39" s="28"/>
-      <c r="H39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="26"/>
+      <c r="I39" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="21">
         <v>43210</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
+      <c r="C40" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="D40" s="42"/>
       <c r="E40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="26"/>
+      <c r="F40" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" s="43"/>
+      <c r="H40" s="42"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F41" s="2"/>
@@ -1557,17 +1576,52 @@
     </row>
   </sheetData>
   <mergeCells count="73">
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="F36:H36"/>
+    <mergeCell ref="F37:H37"/>
+    <mergeCell ref="F38:H38"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="F40:H40"/>
+    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="F28:H28"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="F24:H24"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="F26:H26"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F11:H11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="F29:H29"/>
@@ -1584,52 +1638,17 @@
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="F24:H24"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="F26:H26"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="F28:H28"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="F36:H36"/>
-    <mergeCell ref="F37:H37"/>
-    <mergeCell ref="F38:H38"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="F40:H40"/>
-    <mergeCell ref="C35:E36"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5:H5" r:id="rId1" display="Accessible ici"/>

</xml_diff>